<commit_message>
Add extracting date from URL functionality to Reading Nutritions and Calories sequence
</commit_message>
<xml_diff>
--- a/Data/Nutritions Data.xlsx
+++ b/Data/Nutritions Data.xlsx
@@ -1,71 +1,155 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-  </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15">
+  <x:fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <x:workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
+  <x:bookViews>
+    <x:workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="0" activeTab="0"/>
+  </x:bookViews>
+  <x:sheets>
+    <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+  </x:sheets>
+  <x:definedNames/>
+  <x:calcPr calcId="162913"/>
+  <x:extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
-</workbook>
+    </x:ext>
+  </x:extLst>
+</x:workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+  <x:si>
+    <x:t>10/28/2023</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1498</x:t>
+  </x:si>
+  <x:si>
+    <x:t>51.2 g</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0 g</x:t>
+  </x:si>
+  <x:si>
+    <x:t>103.5 g</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1863.2 mg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>152.4 g</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Daily Calorie Composition: 28% from carbs, 31% from fat and 41% from protein.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10/29/2023</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1492</x:t>
+  </x:si>
+  <x:si>
+    <x:t>46.5 g</x:t>
+  </x:si>
+  <x:si>
+    <x:t>195 g</x:t>
+  </x:si>
+  <x:si>
+    <x:t>475.7 mg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>73.6 g</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Daily Calorie Composition: 52% from carbs, 28% from fat and 20% from protein.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10/30/2023</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1327</x:t>
+  </x:si>
+  <x:si>
+    <x:t>64.3 g</x:t>
+  </x:si>
+  <x:si>
+    <x:t>109.4 g</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1137.9 mg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>75.6 g</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Daily Calorie Composition: 33% from carbs, 44% from fat and 23% from protein.</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-  </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-  </fills>
-  <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-  </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-  </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-  </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2">
+  <x:numFmts count="1">
+    <x:numFmt numFmtId="0" formatCode=""/>
+  </x:numFmts>
+  <x:fonts count="2" x14ac:knownFonts="1">
+    <x:font>
+      <x:sz val="11"/>
+      <x:color theme="1"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+  </x:fonts>
+  <x:fills count="2">
+    <x:fill>
+      <x:patternFill patternType="none"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="gray125"/>
+    </x:fill>
+  </x:fills>
+  <x:borders count="1">
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
+    </x:border>
+  </x:borders>
+  <x:cellStyleXfs count="1">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </x:cellStyleXfs>
+  <x:cellXfs count="1">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  </x:cellXfs>
+  <x:cellStyles count="1">
+    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </x:cellStyles>
+  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+    </x:ext>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
       <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
-</styleSheet>
+    </x:ext>
+  </x:extLst>
+</x:styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -330,13 +414,108 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:9">
+      <x:c r="A1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F1" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="G1" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H1" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I1" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:9">
+      <x:c r="A2" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E2" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="F2" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="G2" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H2" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I2" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:9">
+      <x:c r="A3" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="F3" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="G3" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="H3" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I3" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>

<commit_message>
Improve Reading Calories And Nutritions Data functionality
</commit_message>
<xml_diff>
--- a/Data/Nutritions Data.xlsx
+++ b/Data/Nutritions Data.xlsx
@@ -20,75 +20,93 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+  <x:si>
+    <x:t>Date</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Calories</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Fat (g)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Fiber (g)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Carbs (g)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sodium (mg)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Protein (g)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Water (ml)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Energy From Carbs</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Energy From Fat</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Energy From Protein</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10/27/2023</x:t>
+  </x:si>
+  <x:si>
+    <x:t>36%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32%</x:t>
+  </x:si>
   <x:si>
     <x:t>10/28/2023</x:t>
   </x:si>
   <x:si>
-    <x:t>1498</x:t>
-  </x:si>
-  <x:si>
-    <x:t>51.2 g</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0 g</x:t>
-  </x:si>
-  <x:si>
-    <x:t>103.5 g</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1863.2 mg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>152.4 g</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Daily Calorie Composition: 28% from carbs, 31% from fat and 41% from protein.</x:t>
+    <x:t>28%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>31%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>41%</x:t>
   </x:si>
   <x:si>
     <x:t>10/29/2023</x:t>
   </x:si>
   <x:si>
-    <x:t>1492</x:t>
-  </x:si>
-  <x:si>
-    <x:t>46.5 g</x:t>
-  </x:si>
-  <x:si>
-    <x:t>195 g</x:t>
-  </x:si>
-  <x:si>
-    <x:t>475.7 mg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>73.6 g</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Daily Calorie Composition: 52% from carbs, 28% from fat and 20% from protein.</x:t>
+    <x:t>52%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>20%</x:t>
   </x:si>
   <x:si>
     <x:t>10/30/2023</x:t>
   </x:si>
   <x:si>
-    <x:t>1327</x:t>
-  </x:si>
-  <x:si>
-    <x:t>64.3 g</x:t>
-  </x:si>
-  <x:si>
-    <x:t>109.4 g</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1137.9 mg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>75.6 g</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Daily Calorie Composition: 33% from carbs, 44% from fat and 23% from protein.</x:t>
+    <x:t>33%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>44%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>23%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10/31/2023</x:t>
+  </x:si>
+  <x:si>
+    <x:t>40%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>26%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>34%</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -424,7 +442,7 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:sheetData>
-    <x:row r="1" spans="1:9">
+    <x:row r="1" spans="1:11">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -452,63 +470,186 @@
       <x:c r="I1" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
+      <x:c r="J1" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="K1" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
     </x:row>
-    <x:row r="2" spans="1:9">
+    <x:row r="2" spans="1:11">
       <x:c r="A2" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="B2" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C2" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="D2" s="0" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="E2" s="0" t="s">
+      <x:c r="B2" s="0" t="n">
+        <x:v>1323</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="n">
+        <x:v>46.1</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E2" s="0" t="n">
+        <x:v>116.2</x:v>
+      </x:c>
+      <x:c r="F2" s="0" t="n">
+        <x:v>1477.6</x:v>
+      </x:c>
+      <x:c r="G2" s="0" t="n">
+        <x:v>105.7</x:v>
+      </x:c>
+      <x:c r="H2" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I2" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="F2" s="0" t="s">
+      <x:c r="J2" s="0" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="G2" s="0" t="s">
+      <x:c r="K2" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:11">
+      <x:c r="A3" s="0" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="H2" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="I2" s="0" t="s">
+      <x:c r="B3" s="0" t="n">
+        <x:v>1498</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="n">
+        <x:v>51.2</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="n">
+        <x:v>103.5</x:v>
+      </x:c>
+      <x:c r="F3" s="0" t="n">
+        <x:v>1863.2</x:v>
+      </x:c>
+      <x:c r="G3" s="0" t="n">
+        <x:v>152.4</x:v>
+      </x:c>
+      <x:c r="H3" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I3" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
+      <x:c r="J3" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="K3" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
     </x:row>
-    <x:row r="3" spans="1:9">
-      <x:c r="A3" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="B3" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="C3" s="0" t="s">
+    <x:row r="4" spans="1:11">
+      <x:c r="A4" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="D3" s="0" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="E3" s="0" t="s">
+      <x:c r="B4" s="0" t="n">
+        <x:v>1492</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="n">
+        <x:v>46.5</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="n">
+        <x:v>195</x:v>
+      </x:c>
+      <x:c r="F4" s="0" t="n">
+        <x:v>475.7</x:v>
+      </x:c>
+      <x:c r="G4" s="0" t="n">
+        <x:v>73.6</x:v>
+      </x:c>
+      <x:c r="H4" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I4" s="0" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="F3" s="0" t="s">
+      <x:c r="J4" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="K4" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="G3" s="0" t="s">
+    </x:row>
+    <x:row r="5" spans="1:11">
+      <x:c r="A5" s="0" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="H3" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="I3" s="0" t="s">
+      <x:c r="B5" s="0" t="n">
+        <x:v>1327</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="n">
+        <x:v>64.3</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="n">
+        <x:v>109.4</x:v>
+      </x:c>
+      <x:c r="F5" s="0" t="n">
+        <x:v>1137.9</x:v>
+      </x:c>
+      <x:c r="G5" s="0" t="n">
+        <x:v>75.6</x:v>
+      </x:c>
+      <x:c r="H5" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I5" s="0" t="s">
         <x:v>22</x:v>
+      </x:c>
+      <x:c r="J5" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="K5" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:11">
+      <x:c r="A6" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="n">
+        <x:v>1304</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="n">
+        <x:v>37.6</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="n">
+        <x:v>129.6</x:v>
+      </x:c>
+      <x:c r="F6" s="0" t="n">
+        <x:v>899.4</x:v>
+      </x:c>
+      <x:c r="G6" s="0" t="n">
+        <x:v>112.2</x:v>
+      </x:c>
+      <x:c r="H6" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I6" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="J6" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="K6" s="0" t="s">
+        <x:v>28</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>